<commit_message>
CompareTrees and Tests wip
--Fixes to removed and added nodes
--Test output improvements
--Cleaned up a some comments
--Added new test case (Eric, V4)
</commit_message>
<xml_diff>
--- a/SDC.Schema.Tests/Test Files/Breat_Testing_Changes_BreastStagingTest2v3.xlsx
+++ b/SDC.Schema.Tests/Test Files/Breat_Testing_Changes_BreastStagingTest2v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5e9525a8c46b6bf7/One Drive Documents/SDC/SDC Git Repo/SDC.Schema/SDC.Schema.Tests/Test Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{4EA516B0-607E-4C4A-BF8B-19DFB1D2DA88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17D590E5-8901-4B67-9466-80F2BC9268CE}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="8_{4EA516B0-607E-4C4A-BF8B-19DFB1D2DA88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5911FB2-8D95-40A0-A0A8-15BD1CF7FA0C}"/>
   <bookViews>
-    <workbookView xWindow="29213" yWindow="1605" windowWidth="22762" windowHeight="11370" xr2:uid="{4FCD0A5E-23A0-4C77-B1FF-FD46247428B4}"/>
+    <workbookView xWindow="4133" yWindow="2340" windowWidth="22762" windowHeight="11498" xr2:uid="{4FCD0A5E-23A0-4C77-B1FF-FD46247428B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>XML File</t>
   </si>
@@ -155,6 +155,27 @@
   </si>
   <si>
     <t>Should we pull in new subNodes with serialized attributes?  Since they are all new with no Previous matches, I am not including them in the test output.</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>Expected Report (Tree, Metadata, Other)</t>
+  </si>
+  <si>
+    <t>Document that non-IET subnodes were removed from nodeA and added to nodeB</t>
+  </si>
+  <si>
+    <t>Document that IET nodes were removed</t>
+  </si>
+  <si>
+    <t>Document that removed IET subnodes change the atributes in metadata panel</t>
+  </si>
+  <si>
+    <t>Document that IET nodes were added</t>
+  </si>
+  <si>
+    <t>Document that an IETnode ID was changed</t>
   </si>
 </sst>
 </file>
@@ -203,13 +224,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -228,6 +247,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -527,172 +550,203 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1495958-C0C4-4731-9F4A-D29557245704}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="78.19921875" customWidth="1"/>
-    <col min="3" max="3" width="18.46484375" customWidth="1"/>
-    <col min="4" max="4" width="24.46484375" customWidth="1"/>
-    <col min="5" max="5" width="18.46484375" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" customWidth="1"/>
-    <col min="7" max="7" width="44.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="41.46484375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.46484375" customWidth="1"/>
+    <col min="7" max="7" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="44.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>43969.100004300002</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>170</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B3" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>59031.100004300002</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>1590</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>55161.100004300002</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>2860</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="I4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B5" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>17</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>4257.1000043000004</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>160</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="B6" t="s">
+    <row r="6" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>20</v>
       </c>
-      <c r="E6">
+      <c r="G6">
         <v>4156.1000043000004</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>34</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="I6" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="B7" t="s">
+    <row r="7" spans="1:9" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="D7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>22</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="I7" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B8" t="s">
+    <row r="8" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>25</v>
       </c>
-      <c r="E8">
+      <c r="G8">
         <v>40718.100004300002</v>
       </c>
-      <c r="G8" t="s">
+      <c r="I8" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="57" x14ac:dyDescent="0.45">
+      <c r="B11" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="57" x14ac:dyDescent="0.45">
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B13" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B14" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B15" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>